<commit_message>
reviewer comments added to figures
</commit_message>
<xml_diff>
--- a/02_PublishedAnalysis/02_hypothesisbasedanalsysis/FungalOTUs_ANCOM.xlsx
+++ b/02_PublishedAnalysis/02_hypothesisbasedanalsysis/FungalOTUs_ANCOM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alal3493/Documents/Projects/DevelopmentalBorealToad/FungalDevData/02_PublishedAnalysis/02_hypothesisbasedanalsysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97E7D4F4-E976-9C43-A423-3B8D71F2E748}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C23CD9F9-7B52-654B-9440-A09F25089938}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4280" yWindow="460" windowWidth="21320" windowHeight="14200" xr2:uid="{6D6EBF28-2558-AC4B-A8B0-1FD81D161F5E}"/>
   </bookViews>
@@ -583,7 +583,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82A5A45D-1885-2B41-A301-7A18C71101B3}">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>

</xml_diff>